<commit_message>
adding the WdgMTrigger configrations
</commit_message>
<xml_diff>
--- a/WDG Stack Configration exercise/AUTOSAR Watchdog Stack Exercise.xlsx
+++ b/WDG Stack Configration exercise/AUTOSAR Watchdog Stack Exercise.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
   <si>
     <t>Trainee Name</t>
   </si>
@@ -202,6 +202,27 @@
   </si>
   <si>
     <t>WdgMInternalTransition_0</t>
+  </si>
+  <si>
+    <t>WdgMTriggerConditionValue</t>
+  </si>
+  <si>
+    <t>WdgMWatchdogMode</t>
+  </si>
+  <si>
+    <t>WdgMTriggerWatchdogRef</t>
+  </si>
+  <si>
+    <t>WdgMTrigger_0</t>
+  </si>
+  <si>
+    <t>WdgMTrigger_1</t>
+  </si>
+  <si>
+    <t>WdgMWatchdog_0</t>
+  </si>
+  <si>
+    <t>WDGIF_SLOW_MODE</t>
   </si>
 </sst>
 </file>
@@ -870,7 +891,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -902,14 +923,21 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="3" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -940,11 +968,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -972,29 +1000,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1002,16 +1015,29 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="3" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1234,10 +1260,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:E31"/>
+  <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1250,20 +1276,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
     </row>
     <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1272,10 +1298,10 @@
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="31"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1286,10 +1312,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="31"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1324,10 +1350,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="31"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1355,30 +1381,30 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="D20" s="41" t="s">
+      <c r="B20" s="43"/>
+      <c r="D20" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="42"/>
+      <c r="E20" s="45"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43"/>
-      <c r="B21" s="44"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="44"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="D22" s="27" t="s">
+      <c r="B22" s="33"/>
+      <c r="D22" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="28"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
@@ -1423,7 +1449,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="28" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -1435,34 +1461,78 @@
       <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="26" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="31"/>
       <c r="C29" s="5"/>
+      <c r="D29" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="71"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="73"/>
       <c r="C30" s="5"/>
+      <c r="D30" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="73"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="73" t="s">
+        <v>52</v>
+      </c>
       <c r="C31" s="5"/>
+      <c r="D31" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="73" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" location="'SE1'!A1" display="WdgMSupervisedEntity_0"/>
@@ -1491,20 +1561,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="50"/>
+      <c r="B3" s="53"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1539,14 +1609,14 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="55"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="59"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="53"/>
     </row>
     <row r="10" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -1561,10 +1631,10 @@
       <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="33"/>
     </row>
     <row r="13" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
@@ -1575,14 +1645,14 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
-      <c r="B14" s="58"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="49"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="31"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1625,10 +1695,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="48"/>
+      <c r="B23" s="51"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
@@ -1663,10 +1733,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="30"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1680,22 +1750,22 @@
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="27" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" location="WdgMCheckpoint_0" display="WdgMCheckpoint_0"/>
@@ -1724,20 +1794,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="64"/>
     </row>
     <row r="2" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="33"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -1756,7 +1826,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -1764,7 +1834,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="70"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="20" t="s">
         <v>37</v>
       </c>
@@ -1778,14 +1848,14 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
-      <c r="B9" s="63"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="69"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="33"/>
     </row>
     <row r="11" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
@@ -1796,14 +1866,14 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55"/>
-      <c r="B12" s="56"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="59"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="61"/>
+      <c r="B13" s="67"/>
     </row>
     <row r="14" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
@@ -1814,14 +1884,14 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
-      <c r="B15" s="56"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="61"/>
+      <c r="B16" s="67"/>
     </row>
     <row r="17" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
@@ -1832,14 +1902,14 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="55"/>
-      <c r="B18" s="56"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="61"/>
+      <c r="B19" s="67"/>
     </row>
     <row r="20" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
@@ -1850,15 +1920,15 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="59"/>
-      <c r="B21" s="60"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="66"/>
     </row>
     <row r="22" spans="1:2" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="48"/>
+      <c r="B24" s="51"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
@@ -1869,7 +1939,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="60" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -1877,16 +1947,16 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="69"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="20" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="30"/>
+      <c r="B30" s="31"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">

</xml_diff>